<commit_message>
explanations for velocity difference
</commit_message>
<xml_diff>
--- a/excelFiles/powerRPM.xlsx
+++ b/excelFiles/powerRPM.xlsx
@@ -19,16 +19,16 @@
     <t>RPM</t>
   </si>
   <si>
-    <t>n = 2</t>
-  </si>
-  <si>
-    <t>n = 4</t>
-  </si>
-  <si>
     <t>n = 6</t>
   </si>
   <si>
     <t>n = 8</t>
+  </si>
+  <si>
+    <t>n = 10</t>
+  </si>
+  <si>
+    <t>n = 12</t>
   </si>
 </sst>
 </file>
@@ -417,16 +417,16 @@
         <v>250</v>
       </c>
       <c r="C2">
-        <v>31.92798079342035</v>
+        <v>31.4320790514329</v>
       </c>
       <c r="D2">
-        <v>31.93401119633798</v>
+        <v>31.08609115878535</v>
       </c>
       <c r="E2">
-        <v>31.4320790514329</v>
+        <v>30.86263554533106</v>
       </c>
       <c r="F2">
-        <v>31.08609115878535</v>
+        <v>30.71145097659952</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -437,16 +437,16 @@
         <v>300</v>
       </c>
       <c r="C3">
-        <v>37.85457371345002</v>
+        <v>37.45977808631555</v>
       </c>
       <c r="D3">
-        <v>37.98958559528164</v>
+        <v>37.08621590197729</v>
       </c>
       <c r="E3">
-        <v>37.45977808631555</v>
+        <v>36.8441935575653</v>
       </c>
       <c r="F3">
-        <v>37.08621590197729</v>
+        <v>36.68051362227827</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -457,16 +457,16 @@
         <v>350</v>
       </c>
       <c r="C4">
-        <v>43.62816573277009</v>
+        <v>43.40123821084231</v>
       </c>
       <c r="D4">
-        <v>43.93475038169198</v>
+        <v>43.0139761525169</v>
       </c>
       <c r="E4">
-        <v>43.40123821084231</v>
+        <v>42.76209520688412</v>
       </c>
       <c r="F4">
-        <v>43.0139761525169</v>
+        <v>42.59183372149599</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -477,16 +477,16 @@
         <v>400</v>
       </c>
       <c r="C5">
-        <v>49.24875658030791</v>
+        <v>49.25645941681119</v>
       </c>
       <c r="D5">
-        <v>49.76950579561673</v>
+        <v>48.86937190972969</v>
       </c>
       <c r="E5">
-        <v>49.25645941681119</v>
+        <v>48.6163404545799</v>
       </c>
       <c r="F5">
-        <v>48.86937190972969</v>
+        <v>48.44541134498705</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -497,16 +497,16 @@
         <v>450</v>
       </c>
       <c r="C6">
-        <v>54.71634630966091</v>
+        <v>55.02544170623519</v>
       </c>
       <c r="D6">
-        <v>55.49385183347314</v>
+        <v>54.65240316824902</v>
       </c>
       <c r="E6">
-        <v>55.02544170623519</v>
+        <v>54.40692939310782</v>
       </c>
       <c r="F6">
-        <v>54.65240316824902</v>
+        <v>54.24124644214601</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -517,16 +517,16 @@
         <v>500</v>
       </c>
       <c r="C7">
-        <v>60.03093497459159</v>
+        <v>60.70818506790365</v>
       </c>
       <c r="D7">
-        <v>61.10778849730784</v>
+        <v>60.36306994809718</v>
       </c>
       <c r="E7">
-        <v>60.70818506790365</v>
+        <v>60.13386196663048</v>
       </c>
       <c r="F7">
-        <v>60.36306994809718</v>
+        <v>59.9793390400714</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -537,16 +537,16 @@
         <v>550</v>
       </c>
       <c r="C8">
-        <v>65.19252254658893</v>
+        <v>66.3046895110965</v>
       </c>
       <c r="D8">
-        <v>66.61131577483464</v>
+        <v>66.00137223886577</v>
       </c>
       <c r="E8">
-        <v>66.3046895110965</v>
+        <v>65.79713819344214</v>
       </c>
       <c r="F8">
-        <v>66.00137223886577</v>
+        <v>65.65968906133061</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -557,16 +557,16 @@
         <v>600</v>
       </c>
       <c r="C9">
-        <v>70.20110903691223</v>
+        <v>71.81495503297286</v>
       </c>
       <c r="D9">
-        <v>72.00443370725174</v>
+        <v>71.56731005716098</v>
       </c>
       <c r="E9">
-        <v>71.81495503297286</v>
+        <v>71.39675807820559</v>
       </c>
       <c r="F9">
-        <v>71.56731005716098</v>
+        <v>71.28229679454765</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -577,16 +577,16 @@
         <v>650</v>
       </c>
       <c r="C10">
-        <v>75.05669452245209</v>
+        <v>77.23898164927799</v>
       </c>
       <c r="D10">
-        <v>77.28714227737413</v>
+        <v>77.06088337711586</v>
       </c>
       <c r="E10">
-        <v>77.23898164927799</v>
+        <v>76.93272152828699</v>
       </c>
       <c r="F10">
-        <v>77.06088337711586</v>
+        <v>76.84716195188679</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -597,16 +597,16 @@
         <v>700</v>
       </c>
       <c r="C11">
-        <v>79.75927893261515</v>
+        <v>82.57676935421584</v>
       </c>
       <c r="D11">
-        <v>82.45944148928599</v>
+        <v>82.48209223230585</v>
       </c>
       <c r="E11">
-        <v>82.57676935421584</v>
+        <v>82.40502877036839</v>
       </c>
       <c r="F11">
-        <v>82.48209223230585</v>
+        <v>82.35428461262575</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -617,16 +617,16 @@
         <v>750</v>
       </c>
       <c r="C12">
-        <v>84.30886231753944</v>
+        <v>87.82831817809721</v>
       </c>
       <c r="D12">
-        <v>87.52133132522451</v>
+        <v>87.8309366144999</v>
       </c>
       <c r="E12">
-        <v>87.82831817809721</v>
+        <v>87.81367966612827</v>
       </c>
       <c r="F12">
-        <v>87.8309366144999</v>
+        <v>87.80366462575816</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -637,16 +637,16 @@
         <v>800</v>
       </c>
       <c r="C13">
-        <v>88.7054446086748</v>
+        <v>92.99362811398348</v>
       </c>
       <c r="D13">
-        <v>92.47281180756923</v>
+        <v>93.10741658373006</v>
       </c>
       <c r="E13">
-        <v>92.99362811398348</v>
+        <v>93.15867422769364</v>
       </c>
       <c r="F13">
-        <v>93.10741658373006</v>
+        <v>93.19530235091173</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -657,16 +657,16 @@
         <v>850</v>
       </c>
       <c r="C14">
-        <v>92.94902509775734</v>
+        <v>98.07269913957506</v>
       </c>
       <c r="D14">
-        <v>97.31388293010488</v>
+        <v>98.31153207946515</v>
       </c>
       <c r="E14">
-        <v>98.07269913957506</v>
+        <v>98.44001160014072</v>
       </c>
       <c r="F14">
-        <v>98.31153207946515</v>
+        <v>98.52919694956744</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -677,16 +677,16 @@
         <v>900</v>
       </c>
       <c r="C15">
-        <v>97.03960518338975</v>
+        <v>103.0655304525748</v>
       </c>
       <c r="D15">
-        <v>102.0445431820434</v>
+        <v>103.4432821345368</v>
       </c>
       <c r="E15">
-        <v>103.0655304525748</v>
+        <v>103.6576933898101</v>
       </c>
       <c r="F15">
-        <v>103.4432821345368</v>
+        <v>103.8053492987544</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -697,16 +697,16 @@
         <v>950</v>
       </c>
       <c r="C16">
-        <v>100.9771841713374</v>
+        <v>107.9721235944897</v>
       </c>
       <c r="D16">
-        <v>106.6647962191466</v>
+        <v>108.5026685205297</v>
       </c>
       <c r="E16">
-        <v>107.9721235944897</v>
+        <v>108.8117188308289</v>
       </c>
       <c r="F16">
-        <v>108.5026685205297</v>
+        <v>109.0237596436829</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -717,16 +717,16 @@
         <v>1000</v>
       </c>
       <c r="C17">
-        <v>104.7617620962124</v>
+        <v>112.7924777846302</v>
       </c>
       <c r="D17">
-        <v>111.1746391283685</v>
+        <v>113.4896904226553</v>
       </c>
       <c r="E17">
-        <v>112.7924777846302</v>
+        <v>113.9020875984793</v>
       </c>
       <c r="F17">
-        <v>113.4896904226553</v>
+        <v>114.1844273401761</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -737,16 +737,16 @@
         <v>1050</v>
       </c>
       <c r="C18">
-        <v>108.3933389601417</v>
+        <v>117.5265930536289</v>
       </c>
       <c r="D18">
-        <v>115.5740726409492</v>
+        <v>118.4043478193855</v>
       </c>
       <c r="E18">
-        <v>117.5265930536289</v>
+        <v>118.9288003208822</v>
       </c>
       <c r="F18">
-        <v>118.4043478193855</v>
+        <v>119.2873524501306</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -757,16 +757,16 @@
         <v>1100</v>
       </c>
       <c r="C19">
-        <v>111.8719147659374</v>
+        <v>122.1744693252922</v>
       </c>
       <c r="D19">
-        <v>119.8630966615673</v>
+        <v>123.2466404828924</v>
       </c>
       <c r="E19">
-        <v>122.1744693252922</v>
+        <v>123.891856713006</v>
       </c>
       <c r="F19">
-        <v>123.2466404828924</v>
+        <v>124.3325352319543</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,16 +777,16 @@
         <v>1150</v>
       </c>
       <c r="C20">
-        <v>115.1974894383087</v>
+        <v>126.7361066386813</v>
       </c>
       <c r="D20">
-        <v>124.0417113113679</v>
+        <v>128.0165690200606</v>
       </c>
       <c r="E20">
-        <v>126.7361066386813</v>
+        <v>128.7912567289297</v>
       </c>
       <c r="F20">
-        <v>128.0165690200606</v>
+        <v>129.3199716532763</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,16 +797,16 @@
         <v>1200</v>
       </c>
       <c r="C21">
-        <v>118.37006343668</v>
+        <v>131.2115049156261</v>
       </c>
       <c r="D21">
-        <v>128.1099166486464</v>
+        <v>132.7141329949274</v>
       </c>
       <c r="E21">
-        <v>131.2115049156261</v>
+        <v>133.6270004666489</v>
       </c>
       <c r="F21">
-        <v>132.7141329949274</v>
+        <v>134.2496687098305</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -817,16 +817,16 @@
         <v>1250</v>
       </c>
       <c r="C22">
-        <v>121.3896363506848</v>
+        <v>135.6006643526352</v>
       </c>
       <c r="D22">
-        <v>132.0677126614094</v>
+        <v>137.339332465151</v>
       </c>
       <c r="E22">
-        <v>135.6006643526352</v>
+        <v>138.399083372868</v>
       </c>
       <c r="F22">
-        <v>137.339332465151</v>
+        <v>139.1216231120662</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -837,16 +837,16 @@
         <v>1300</v>
       </c>
       <c r="C23">
-        <v>124.2562081976853</v>
+        <v>139.9035850886974</v>
       </c>
       <c r="D23">
-        <v>135.9150993873858</v>
+        <v>141.892167649374</v>
       </c>
       <c r="E23">
-        <v>139.9035850886974</v>
+        <v>143.1075133028127</v>
       </c>
       <c r="F23">
-        <v>141.892167649374</v>
+        <v>143.935835115</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -857,16 +857,16 @@
         <v>1350</v>
       </c>
       <c r="C24">
-        <v>126.9697790038321</v>
+        <v>144.1202667643482</v>
       </c>
       <c r="D24">
-        <v>139.6520767514164</v>
+        <v>146.3726380845965</v>
       </c>
       <c r="E24">
-        <v>144.1202667643482</v>
+        <v>147.7522870216128</v>
       </c>
       <c r="F24">
-        <v>146.3726380845965</v>
+        <v>148.6923042116984</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -877,16 +877,16 @@
         <v>1400</v>
       </c>
       <c r="C25">
-        <v>129.5303486496245</v>
+        <v>148.2507095024737</v>
       </c>
       <c r="D25">
-        <v>143.2786447801532</v>
+        <v>150.7807435548122</v>
       </c>
       <c r="E25">
-        <v>148.2507095024737</v>
+        <v>152.333404220209</v>
       </c>
       <c r="F25">
-        <v>150.7807435548122</v>
+        <v>153.391030773999</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -897,16 +897,16 @@
         <v>1450</v>
       </c>
       <c r="C26">
-        <v>131.9379168055217</v>
+        <v>152.2949131919559</v>
       </c>
       <c r="D26">
-        <v>146.794803138704</v>
+        <v>155.1164850560552</v>
       </c>
       <c r="E26">
-        <v>152.2949131919559</v>
+        <v>156.8508654849765</v>
       </c>
       <c r="F26">
-        <v>155.1164850560552</v>
+        <v>158.0320147196015</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -917,16 +917,16 @@
         <v>1500</v>
       </c>
       <c r="C27">
-        <v>134.1924837540811</v>
+        <v>156.2528778902629</v>
       </c>
       <c r="D27">
-        <v>150.2005521860349</v>
+        <v>159.3798619213699</v>
       </c>
       <c r="E27">
-        <v>156.2528778902629</v>
+        <v>161.3046704877619</v>
       </c>
       <c r="F27">
-        <v>159.3798619213699</v>
+        <v>162.6152564844355</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -937,16 +937,16 @@
         <v>1550</v>
       </c>
       <c r="C28">
-        <v>136.2940504057366</v>
+        <v>160.124601226142</v>
       </c>
       <c r="D28">
-        <v>153.4958907567086</v>
+        <v>163.5708718457493</v>
       </c>
       <c r="E28">
-        <v>160.124601226142</v>
+        <v>165.6948191861233</v>
       </c>
       <c r="F28">
-        <v>163.5708718457493</v>
+        <v>167.1407557810563</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -957,16 +957,16 @@
         <v>1600</v>
       </c>
       <c r="C29">
-        <v>138.2426146145497</v>
+        <v>163.9100892760356</v>
       </c>
       <c r="D29">
-        <v>156.6808210836776</v>
+        <v>167.6895205579963</v>
       </c>
       <c r="E29">
-        <v>163.9100892760356</v>
+        <v>170.0213110069543</v>
       </c>
       <c r="F29">
-        <v>167.6895205579963</v>
+        <v>171.6085132037561</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -977,16 +977,16 @@
         <v>1650</v>
       </c>
       <c r="C30">
-        <v>140.0381764670787</v>
+        <v>167.6093373002896</v>
       </c>
       <c r="D30">
-        <v>159.7553442888185</v>
+        <v>171.7358023225276</v>
       </c>
       <c r="E30">
-        <v>167.6093373002896</v>
+        <v>174.284147388448</v>
       </c>
       <c r="F30">
-        <v>171.7358023225276</v>
+        <v>176.0185277172474</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -997,16 +997,16 @@
         <v>1700</v>
       </c>
       <c r="C31">
-        <v>141.6807354995891</v>
+        <v>171.222346548846</v>
       </c>
       <c r="D31">
-        <v>162.7194554722379</v>
+        <v>175.7097183217266</v>
       </c>
       <c r="E31">
-        <v>171.222346548846</v>
+        <v>178.4833279608055</v>
       </c>
       <c r="F31">
-        <v>175.7097183217266</v>
+        <v>180.3707970456744</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1017,16 +1017,16 @@
         <v>1750</v>
       </c>
       <c r="C32">
-        <v>143.1702963620898</v>
+        <v>174.7491158039905</v>
       </c>
       <c r="D32">
-        <v>165.5731574085681</v>
+        <v>179.6112744400351</v>
       </c>
       <c r="E32">
-        <v>174.7491158039905</v>
+        <v>182.6188490085577</v>
       </c>
       <c r="F32">
-        <v>179.6112744400351</v>
+        <v>184.6653270892631</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1037,16 +1037,16 @@
         <v>1800</v>
       </c>
       <c r="C33">
-        <v>144.5068591879525</v>
+        <v>178.1896460553314</v>
       </c>
       <c r="D33">
-        <v>168.316446373777</v>
+        <v>183.4404636078882</v>
       </c>
       <c r="E33">
-        <v>178.1896460553314</v>
+        <v>186.6907242664</v>
       </c>
       <c r="F33">
-        <v>183.4404636078882</v>
+        <v>188.9021147955749</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1057,16 +1057,16 @@
         <v>1850</v>
       </c>
       <c r="C34">
-        <v>145.6904185735209</v>
+        <v>181.5439353940317</v>
       </c>
       <c r="D34">
-        <v>170.9493277989533</v>
+        <v>187.1972896990819</v>
       </c>
       <c r="E34">
-        <v>181.5439353940317</v>
+        <v>190.6989342798495</v>
       </c>
       <c r="F34">
-        <v>187.1972896990819</v>
+        <v>193.0811674958335</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1077,16 +1077,16 @@
         <v>1900</v>
       </c>
       <c r="C35">
-        <v>146.7209767321476</v>
+        <v>184.8119878721801</v>
       </c>
       <c r="D35">
-        <v>173.471797536011</v>
+        <v>190.881745005936</v>
       </c>
       <c r="E35">
-        <v>184.8119878721801</v>
+        <v>194.6434881873882</v>
       </c>
       <c r="F35">
-        <v>190.881745005936</v>
+        <v>197.2024676475269</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1097,16 +1097,16 @@
         <v>1950</v>
       </c>
       <c r="C36">
-        <v>147.598533424419</v>
+        <v>187.9938027851284</v>
       </c>
       <c r="D36">
-        <v>175.8838597632305</v>
+        <v>194.4938407934023</v>
       </c>
       <c r="E36">
-        <v>187.9938027851284</v>
+        <v>198.5243753669275</v>
       </c>
       <c r="F36">
-        <v>194.4938407934023</v>
+        <v>201.2660137141443</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1117,16 +1117,16 @@
         <v>2000</v>
       </c>
       <c r="C37">
-        <v>148.3230891455013</v>
+        <v>191.089376154662</v>
       </c>
       <c r="D37">
-        <v>178.1855193156488</v>
+        <v>198.033568678983</v>
       </c>
       <c r="E37">
-        <v>191.089376154662</v>
+        <v>202.3416152353407</v>
       </c>
       <c r="F37">
-        <v>198.033568678983</v>
+        <v>205.2718308750261</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1137,16 +1137,16 @@
         <v>2050</v>
       </c>
       <c r="C38">
-        <v>148.8946439045644</v>
+        <v>194.0987135911171</v>
       </c>
       <c r="D38">
-        <v>180.3767627310321</v>
+        <v>201.5009437193125</v>
       </c>
       <c r="E38">
-        <v>194.0987135911171</v>
+        <v>206.0952091081971</v>
       </c>
       <c r="F38">
-        <v>201.5009437193125</v>
+        <v>209.219912544971</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1157,16 +1157,16 @@
         <v>2100</v>
       </c>
       <c r="C39">
-        <v>149.3131973816353</v>
+        <v>197.0218107648976</v>
       </c>
       <c r="D39">
-        <v>182.4576041918715</v>
+        <v>204.895947734788</v>
       </c>
       <c r="E39">
-        <v>197.0218107648976</v>
+        <v>209.7851384109113</v>
       </c>
       <c r="F39">
-        <v>204.895947734788</v>
+        <v>213.1102463031717</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1177,16 +1177,16 @@
         <v>2150</v>
       </c>
       <c r="C40">
-        <v>149.5787492033743</v>
+        <v>199.8586690687258</v>
       </c>
       <c r="D40">
-        <v>184.4280310854321</v>
+        <v>208.21858237973</v>
       </c>
       <c r="E40">
-        <v>199.8586690687258</v>
+        <v>213.4114117861577</v>
       </c>
       <c r="F40">
-        <v>208.21858237973</v>
+        <v>216.9428361419226</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1197,16 +1197,16 @@
         <v>2200</v>
       </c>
       <c r="C41">
-        <v>149.6913000325726</v>
+        <v>202.609288368359</v>
       </c>
       <c r="D41">
-        <v>186.2880486759868</v>
+        <v>211.4688564427171</v>
       </c>
       <c r="E41">
-        <v>202.609288368359</v>
+        <v>216.9740237036303</v>
       </c>
       <c r="F41">
-        <v>211.4688564427171</v>
+        <v>220.7176845632928</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1217,16 +1217,16 @@
         <v>2250</v>
       </c>
       <c r="C42">
-        <v>149.6508493062546</v>
+        <v>205.2736687062037</v>
       </c>
       <c r="D42">
-        <v>188.0376566201535</v>
+        <v>214.6467658595484</v>
       </c>
       <c r="E42">
-        <v>205.2736687062037</v>
+        <v>220.4729828329763</v>
       </c>
       <c r="F42">
-        <v>214.6467658595484</v>
+        <v>224.4347892310888</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1237,16 +1237,16 @@
         <v>2300</v>
       </c>
       <c r="C43">
-        <v>149.4574082059158</v>
+        <v>207.8518101975736</v>
       </c>
       <c r="D43">
-        <v>189.6768551737595</v>
+        <v>217.75230875749</v>
       </c>
       <c r="E43">
-        <v>207.8518101975736</v>
+        <v>223.9082861430476</v>
       </c>
       <c r="F43">
-        <v>217.75230875749</v>
+        <v>228.0941467506828</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1257,16 +1257,16 @@
         <v>2350</v>
       </c>
       <c r="C44">
-        <v>149.1109566988465</v>
+        <v>210.3437125893837</v>
       </c>
       <c r="D44">
-        <v>191.2056444654915</v>
+        <v>220.7854886101773</v>
       </c>
       <c r="E44">
-        <v>210.3437125893837</v>
+        <v>227.2799331879871</v>
       </c>
       <c r="F44">
-        <v>220.7854886101773</v>
+        <v>231.695765701633</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1277,16 +1277,16 @@
         <v>2400</v>
       </c>
       <c r="C45">
-        <v>148.6115040567247</v>
+        <v>212.749376218879</v>
       </c>
       <c r="D45">
-        <v>192.624024236534</v>
+        <v>223.7463043431237</v>
       </c>
       <c r="E45">
-        <v>212.749376218879</v>
+        <v>230.5879240380927</v>
       </c>
       <c r="F45">
-        <v>223.7463043431237</v>
+        <v>235.2396424638745</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1297,16 +1297,16 @@
         <v>2450</v>
       </c>
       <c r="C46">
-        <v>147.9590501605172</v>
+        <v>215.0688007749123</v>
       </c>
       <c r="D46">
-        <v>193.9319948089697</v>
+        <v>226.6347553147518</v>
       </c>
       <c r="E46">
-        <v>215.0688007749123</v>
+        <v>233.8322557867167</v>
       </c>
       <c r="F46">
-        <v>226.6347553147518</v>
+        <v>238.7257765873849</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1317,16 +1317,16 @@
         <v>2500</v>
       </c>
       <c r="C47">
-        <v>147.1535956383794</v>
+        <v>217.3019864139662</v>
       </c>
       <c r="D47">
-        <v>195.129555848962</v>
+        <v>229.4508421181654</v>
       </c>
       <c r="E47">
-        <v>217.3019864139662</v>
+        <v>237.0129311370346</v>
       </c>
       <c r="F47">
-        <v>229.4508421181654</v>
+        <v>242.154168363733</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1337,16 +1337,16 @@
         <v>2550</v>
       </c>
       <c r="C48">
-        <v>146.1951397048369</v>
+        <v>219.4489332807905</v>
       </c>
       <c r="D48">
-        <v>196.2167077682379</v>
+        <v>232.1945640964346</v>
       </c>
       <c r="E48">
-        <v>219.4489332807905</v>
+        <v>240.1299522957436</v>
       </c>
       <c r="F48">
-        <v>232.1945640964346</v>
+        <v>245.5248177473365</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1357,16 +1357,16 @@
         <v>2600</v>
       </c>
       <c r="C49">
-        <v>145.0836827086267</v>
+        <v>221.509641132402</v>
       </c>
       <c r="D49">
-        <v>197.1934500325938</v>
+        <v>234.8659216048125</v>
       </c>
       <c r="E49">
-        <v>221.509641132402</v>
+        <v>243.1833204874445</v>
       </c>
       <c r="F49">
-        <v>234.8659216048125</v>
+        <v>248.8377262270008</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1377,16 +1377,16 @@
         <v>2650</v>
       </c>
       <c r="C50">
-        <v>143.819222312029</v>
+        <v>223.4841100447575</v>
       </c>
       <c r="D50">
-        <v>198.0597828320223</v>
+        <v>237.464914791392</v>
       </c>
       <c r="E50">
-        <v>223.4841100447575</v>
+        <v>246.1730292450643</v>
       </c>
       <c r="F50">
-        <v>237.464914791392</v>
+        <v>252.0928867503094</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1397,16 +1397,16 @@
         <v>2700</v>
       </c>
       <c r="C51">
-        <v>142.4017631715849</v>
+        <v>225.3723399975419</v>
       </c>
       <c r="D51">
-        <v>198.8157060499891</v>
+        <v>239.9915429076291</v>
       </c>
       <c r="E51">
-        <v>225.3723399975419</v>
+        <v>249.0990814892138</v>
       </c>
       <c r="F51">
-        <v>239.9915429076291</v>
+        <v>255.2903097694698</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1417,16 +1417,16 @@
         <v>2750</v>
       </c>
       <c r="C52">
-        <v>140.8313029478921</v>
+        <v>227.1743307591319</v>
       </c>
       <c r="D52">
-        <v>199.4612195795209</v>
+        <v>242.445806462874</v>
       </c>
       <c r="E52">
-        <v>227.1743307591319</v>
+        <v>251.9614770213304</v>
       </c>
       <c r="F52">
-        <v>242.445806462874</v>
+        <v>258.42998833812</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1437,16 +1437,16 @@
         <v>2800</v>
       </c>
       <c r="C53">
-        <v>139.1078416538815</v>
+        <v>228.8900824399083</v>
       </c>
       <c r="D53">
-        <v>199.9963240263653</v>
+        <v>244.8277051708988</v>
       </c>
       <c r="E53">
-        <v>228.8900824399083</v>
+        <v>254.7602161345295</v>
       </c>
       <c r="F53">
-        <v>244.8277051708988</v>
+        <v>261.5119243693097</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1457,16 +1457,16 @@
         <v>2850</v>
       </c>
       <c r="C54">
-        <v>137.2313632198001</v>
+        <v>230.5195951985102</v>
       </c>
       <c r="D54">
-        <v>200.4210193662582</v>
+        <v>247.137239745749</v>
       </c>
       <c r="E54">
-        <v>230.5195951985102</v>
+        <v>257.4952988464188</v>
       </c>
       <c r="F54">
-        <v>247.137239745749</v>
+        <v>264.5361178435624</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1477,16 +1477,16 @@
         <v>2900</v>
       </c>
       <c r="C55">
-        <v>135.2018989149898</v>
+        <v>232.0628690309526</v>
       </c>
       <c r="D55">
-        <v>200.7353049137796</v>
+        <v>249.3744094331901</v>
       </c>
       <c r="E55">
-        <v>232.0628690309526</v>
+        <v>260.1667251991854</v>
       </c>
       <c r="F55">
-        <v>249.3744094331901</v>
+        <v>267.502568758089</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1497,16 +1497,16 @@
         <v>2950</v>
       </c>
       <c r="C56">
-        <v>133.0194338295251</v>
+        <v>233.5199041062582</v>
       </c>
       <c r="D56">
-        <v>200.9391810183336</v>
+        <v>251.5392146278699</v>
       </c>
       <c r="E56">
-        <v>233.5199041062582</v>
+        <v>262.7744952008401</v>
       </c>
       <c r="F56">
-        <v>251.5392146278699</v>
+        <v>270.4112771337622</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1517,16 +1517,16 @@
         <v>3000</v>
       </c>
       <c r="C57">
-        <v>130.6839676686421</v>
+        <v>234.89070044421</v>
       </c>
       <c r="D57">
-        <v>201.0326480340901</v>
+        <v>253.6316521655377</v>
       </c>
       <c r="E57">
-        <v>234.89070044421</v>
+        <v>265.3186088564652</v>
       </c>
       <c r="F57">
-        <v>253.6316521655377</v>
+        <v>273.2622429770296</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1537,16 +1537,16 @@
         <v>3050</v>
       </c>
       <c r="C58">
-        <v>128.1955004307128</v>
+        <v>236.1752576032763</v>
       </c>
       <c r="D58">
-        <v>201.0157053616878</v>
+        <v>255.6517290050141</v>
       </c>
       <c r="E58">
-        <v>236.1752576032763</v>
+        <v>267.7990665973409</v>
       </c>
       <c r="F58">
-        <v>255.6517290050141</v>
+        <v>276.0554662941836</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1557,16 +1557,16 @@
         <v>3100</v>
       </c>
       <c r="C59">
-        <v>125.5540321224326</v>
+        <v>237.3735758978542</v>
       </c>
       <c r="D59">
-        <v>200.8883533280386</v>
+        <v>257.5994408052587</v>
       </c>
       <c r="E59">
-        <v>237.3735758978542</v>
+        <v>270.2158671392444</v>
       </c>
       <c r="F59">
-        <v>257.5994408052587</v>
+        <v>278.7909471171159</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1577,16 +1577,16 @@
         <v>3150</v>
       </c>
       <c r="C60">
-        <v>122.7595626969685</v>
+        <v>238.4856551604135</v>
       </c>
       <c r="D60">
-        <v>200.6505922263768</v>
+        <v>259.4747880701139</v>
       </c>
       <c r="E60">
-        <v>238.4856551604135</v>
+        <v>272.5690112548382</v>
       </c>
       <c r="F60">
-        <v>259.4747880701139</v>
+        <v>281.4686854495732</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1597,16 +1597,16 @@
         <v>3200</v>
       </c>
       <c r="C61">
-        <v>119.8120918292701</v>
+        <v>239.5114956028826</v>
       </c>
       <c r="D61">
-        <v>200.3024214321484</v>
+        <v>261.2777707172247</v>
       </c>
       <c r="E61">
-        <v>239.5114956028826</v>
+        <v>274.8584994726169</v>
       </c>
       <c r="F61">
-        <v>261.2777707172247</v>
+        <v>284.0886810857929</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1617,16 +1617,16 @@
         <v>3250</v>
       </c>
       <c r="C62">
-        <v>116.7116197763461</v>
+        <v>240.4510971014994</v>
       </c>
       <c r="D62">
-        <v>199.8438412634905</v>
+        <v>263.0083888611036</v>
       </c>
       <c r="E62">
-        <v>240.4510971014994</v>
+        <v>277.0843308678486</v>
       </c>
       <c r="F62">
-        <v>263.0083888611036</v>
+        <v>286.6509342345331</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1637,16 +1637,16 @@
         <v>3300</v>
       </c>
       <c r="C63">
-        <v>113.4581466430135</v>
+        <v>241.304459666664</v>
       </c>
       <c r="D63">
-        <v>199.2748517226239</v>
+        <v>264.6666425937235</v>
       </c>
       <c r="E63">
-        <v>241.304459666664</v>
+        <v>279.2465061357764</v>
       </c>
       <c r="F63">
-        <v>264.6666425937235</v>
+        <v>289.1554448315322</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1657,16 +1657,16 @@
         <v>3350</v>
       </c>
       <c r="C64">
-        <v>110.051672429182</v>
+        <v>242.0715832065334</v>
       </c>
       <c r="D64">
-        <v>198.5954531190095</v>
+        <v>266.2525319812474</v>
       </c>
       <c r="E64">
-        <v>242.0715832065334</v>
+        <v>281.3450245028831</v>
       </c>
       <c r="F64">
-        <v>266.2525319812474</v>
+        <v>291.6022131583036</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1677,16 +1677,16 @@
         <v>3400</v>
       </c>
       <c r="C65">
-        <v>106.4921975843143</v>
+        <v>242.7524678971625</v>
       </c>
       <c r="D65">
-        <v>197.805644892058</v>
+        <v>267.7660568850614</v>
       </c>
       <c r="E65">
-        <v>242.7524678971625</v>
+        <v>283.3798826370447</v>
       </c>
       <c r="F65">
-        <v>267.7660568850614</v>
+        <v>293.9912384848024</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1697,16 +1697,16 @@
         <v>3450</v>
       </c>
       <c r="C66">
-        <v>102.7797137199868</v>
+        <v>243.3471135633513</v>
       </c>
       <c r="D66">
-        <v>196.9054272867122</v>
+        <v>269.2072173179897</v>
       </c>
       <c r="E66">
-        <v>243.3471135633513</v>
+        <v>285.3510885168906</v>
       </c>
       <c r="F66">
-        <v>269.2072173179897</v>
+        <v>296.3225212444889</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1717,16 +1717,16 @@
         <v>3500</v>
       </c>
       <c r="C67">
-        <v>98.91423625834291</v>
+        <v>243.8555202856368</v>
       </c>
       <c r="D67">
-        <v>195.8948008995274</v>
+        <v>270.5760140999067</v>
       </c>
       <c r="E67">
-        <v>243.8555202856368</v>
+        <v>287.2586380381171</v>
       </c>
       <c r="F67">
-        <v>270.5760140999067</v>
+        <v>298.5960614931753</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1737,16 +1737,16 @@
         <v>3550</v>
       </c>
       <c r="C68">
-        <v>94.89575769361677</v>
+        <v>244.2776880507995</v>
       </c>
       <c r="D68">
-        <v>194.7737646115043</v>
+        <v>271.872445701141</v>
       </c>
       <c r="E68">
-        <v>244.2776880507995</v>
+        <v>289.1025312582394</v>
       </c>
       <c r="F68">
-        <v>271.872445701141</v>
+        <v>300.8118589240315</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1757,16 +1757,16 @@
         <v>3600</v>
       </c>
       <c r="C69">
-        <v>90.72427800626986</v>
+        <v>244.6136168564116</v>
       </c>
       <c r="D69">
-        <v>193.5423189178411</v>
+        <v>273.096512816319</v>
       </c>
       <c r="E69">
-        <v>244.6136168564116</v>
+        <v>290.8827725664149</v>
       </c>
       <c r="F69">
-        <v>273.096512816319</v>
+        <v>302.9699149126276</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1777,16 +1777,16 @@
         <v>3650</v>
       </c>
       <c r="C70">
-        <v>86.39979715289326</v>
+        <v>244.8633067142047</v>
       </c>
       <c r="D70">
-        <v>192.2004638286173</v>
+        <v>274.2482154498801</v>
       </c>
       <c r="E70">
-        <v>244.8633067142047</v>
+        <v>292.599353482514</v>
       </c>
       <c r="F70">
-        <v>274.2482154498801</v>
+        <v>305.070227523808</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1797,16 +1797,16 @@
         <v>3700</v>
       </c>
       <c r="C71">
-        <v>81.92231520686322</v>
+        <v>245.0267576217876</v>
       </c>
       <c r="D71">
-        <v>190.7481993545834</v>
+        <v>275.327553629983</v>
       </c>
       <c r="E71">
-        <v>245.0267576217876</v>
+        <v>294.2522744871238</v>
       </c>
       <c r="F71">
-        <v>275.327553629983</v>
+        <v>307.1127976268084</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1817,16 +1817,16 @@
         <v>3750</v>
       </c>
       <c r="C72">
-        <v>77.29183216646642</v>
+        <v>245.1039695714473</v>
       </c>
       <c r="D72">
-        <v>189.185525496527</v>
+        <v>276.3345273108993</v>
       </c>
       <c r="E72">
-        <v>245.1039695714473</v>
+        <v>295.8415424727809</v>
       </c>
       <c r="F72">
-        <v>276.3345273108993</v>
+        <v>309.0976252275033</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1837,16 +1837,16 @@
         <v>3800</v>
       </c>
       <c r="C73">
-        <v>72.5083480294215</v>
+        <v>245.0949425644876</v>
       </c>
       <c r="D73">
-        <v>187.5124422442793</v>
+        <v>277.2691363114743</v>
       </c>
       <c r="E73">
-        <v>245.0949425644876</v>
+        <v>297.3671482306516</v>
       </c>
       <c r="F73">
-        <v>277.2691363114743</v>
+        <v>311.0247103291948</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1857,16 +1857,16 @@
         <v>3850</v>
       </c>
       <c r="C74">
-        <v>67.57186279378723</v>
+        <v>244.9996771153608</v>
       </c>
       <c r="D74">
-        <v>185.7289495947275</v>
+        <v>278.1313807982491</v>
       </c>
       <c r="E74">
-        <v>244.9996771153608</v>
+        <v>298.8291031079788</v>
       </c>
       <c r="F74">
-        <v>278.1313807982491</v>
+        <v>312.8940529263432</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1877,16 +1877,16 @@
         <v>3900</v>
       </c>
       <c r="C75">
-        <v>62.48237646035913</v>
+        <v>244.8181721954944</v>
       </c>
       <c r="D75">
-        <v>183.8350473505058</v>
+        <v>278.9212607760857</v>
       </c>
       <c r="E75">
-        <v>244.8181721954944</v>
+        <v>300.2274021171849</v>
       </c>
       <c r="F75">
-        <v>278.9212607760857</v>
+        <v>314.7056539301986</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1897,16 +1897,16 @@
         <v>3950</v>
       </c>
       <c r="C76">
-        <v>57.23988902691802</v>
+        <v>244.5504283240808</v>
       </c>
       <c r="D76">
-        <v>181.8307356524658</v>
+        <v>279.6387762541846</v>
       </c>
       <c r="E76">
-        <v>244.5504283240808</v>
+        <v>301.5620441798806</v>
       </c>
       <c r="F76">
-        <v>279.6387762541846</v>
+        <v>316.459511429269</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1917,16 +1917,16 @@
         <v>4000</v>
       </c>
       <c r="C77">
-        <v>51.84440095920146</v>
+        <v>244.1964455041772</v>
       </c>
       <c r="D77">
-        <v>179.7160147200965</v>
+        <v>280.2839272082995</v>
       </c>
       <c r="E77">
-        <v>244.1964455041772</v>
+        <v>302.8330298473712</v>
       </c>
       <c r="F77">
-        <v>280.2839272082995</v>
+        <v>318.1556265038107</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1937,16 +1937,16 @@
         <v>4050</v>
       </c>
       <c r="C78">
-        <v>46.29591128100879</v>
+        <v>243.7562237406937</v>
       </c>
       <c r="D78">
-        <v>177.4908842333843</v>
+        <v>280.8567136205778</v>
       </c>
       <c r="E78">
-        <v>243.7562237406937</v>
+        <v>304.0403591287326</v>
       </c>
       <c r="F78">
-        <v>280.8567136205778</v>
+        <v>319.7940002206379</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1957,16 +1957,16 @@
         <v>4100</v>
       </c>
       <c r="C79">
-        <v>40.59442050594746</v>
+        <v>243.2297629528993</v>
       </c>
       <c r="D79">
-        <v>175.1553443546185</v>
+        <v>281.3571354837072</v>
       </c>
       <c r="E79">
-        <v>243.2297629528993</v>
+        <v>305.1840320320132</v>
       </c>
       <c r="F79">
-        <v>281.3571354837072</v>
+        <v>321.3746306612811</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1977,16 +1977,16 @@
         <v>4150</v>
       </c>
       <c r="C80">
-        <v>34.73992862813429</v>
+        <v>242.6170631906977</v>
       </c>
       <c r="D80">
-        <v>172.7093950826261</v>
+        <v>281.7851927944745</v>
       </c>
       <c r="E80">
-        <v>242.6170631906977</v>
+        <v>306.2640485596816</v>
       </c>
       <c r="F80">
-        <v>281.7851927944745</v>
+        <v>322.8975185903111</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1997,16 +1997,16 @@
         <v>4200</v>
       </c>
       <c r="C81">
-        <v>28.73243565371904</v>
+        <v>241.9181248739352</v>
       </c>
       <c r="D81">
-        <v>170.1530371082718</v>
+        <v>282.1408866811849</v>
       </c>
       <c r="E81">
-        <v>241.9181248739352</v>
+        <v>307.2804087075504</v>
       </c>
       <c r="F81">
-        <v>282.1408866811849</v>
+        <v>324.3626639859814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>